<commit_message>
Added new experiment instead of 7
</commit_message>
<xml_diff>
--- a/plots/experiment7_unconditional.xlsx
+++ b/plots/experiment7_unconditional.xlsx
@@ -564,16 +564,16 @@
         <v>0.108</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9342</v>
+        <v>1.0371</v>
       </c>
       <c r="G4" t="n">
-        <v>0.035</v>
+        <v>2</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9186</v>
+        <v>0.6901</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0069</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -593,16 +593,16 @@
         <v>0.3449</v>
       </c>
       <c r="F5" t="n">
-        <v>0.947</v>
+        <v>1.106</v>
       </c>
       <c r="G5" t="n">
-        <v>0.006</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9989</v>
+        <v>0.8909</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0019</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -617,25 +617,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.0257</v>
+        <v>0.0254</v>
       </c>
       <c r="D6" t="n">
-        <v>111.4</v>
+        <v>76</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3205</v>
+        <v>0.3188</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7688</v>
+        <v>0.4747</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0156</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>134333.7676</v>
+        <v>59276.1261</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0054</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -646,25 +646,25 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.0094</v>
+        <v>0.0097</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1374</v>
+        <v>0.1391</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4491</v>
+        <v>0.4333</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>2.1838</v>
+        <v>2.8263</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0051</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -675,25 +675,25 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.0289</v>
+        <v>0.0291</v>
       </c>
       <c r="D8" t="n">
-        <v>317.8</v>
+        <v>347</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1991</v>
+        <v>0.2006</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3431</v>
+        <v>0.3107</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0064</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>3425.4808</v>
+        <v>2627.2297</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -717,16 +717,16 @@
         <v>0.2651</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4084</v>
+        <v>0.3198</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0453</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>1.5617</v>
+        <v>0.7712</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0214</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -746,16 +746,16 @@
         <v>0.1144</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3816</v>
+        <v>0.4554</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0182</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0.643</v>
+        <v>0.9021</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0725</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -775,16 +775,16 @@
         <v>0.09719999999999999</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5745</v>
+        <v>0.1255</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0095</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>3.4701</v>
+        <v>0.5069</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -804,16 +804,16 @@
         <v>0.3237</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5063</v>
+        <v>0.5141</v>
       </c>
       <c r="G12" t="n">
-        <v>0.008699999999999999</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>0.8915</v>
+        <v>0.8048</v>
       </c>
       <c r="I12" t="n">
-        <v>0.2141</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -831,22 +831,22 @@
         <v>0.0398</v>
       </c>
       <c r="D13" t="n">
-        <v>7.4</v>
+        <v>5</v>
       </c>
       <c r="E13" t="n">
         <v>0.281</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3021</v>
+        <v>0.4341</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0927</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>2.4447</v>
+        <v>3.9187</v>
       </c>
       <c r="I13" t="n">
-        <v>0.06950000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -866,16 +866,16 @@
         <v>0.1172</v>
       </c>
       <c r="F14" t="n">
-        <v>0.534</v>
+        <v>0.4527</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1279</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4856</v>
+        <v>0.4627</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1345</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -895,13 +895,13 @@
         <v>0.0635</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4712</v>
+        <v>0.4989</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0021</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>0.5132</v>
+        <v>0.4639</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -924,16 +924,16 @@
         <v>0.0824</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2456</v>
+        <v>0.2138</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0022</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>2.5402</v>
+        <v>3.2094</v>
       </c>
       <c r="I16" t="n">
-        <v>0.008</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -957,16 +957,16 @@
         <v>0.1482</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3515</v>
+        <v>0.3027</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0223</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>2.9598</v>
+        <v>4.7485</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -986,16 +986,16 @@
         <v>0.4239</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2636</v>
+        <v>0.3181</v>
       </c>
       <c r="G18" t="n">
-        <v>0.048</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>80736.26210000001</v>
+        <v>148069.2947</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0559</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1015,16 +1015,16 @@
         <v>0.1197</v>
       </c>
       <c r="F19" t="n">
-        <v>0.3205</v>
+        <v>0.3489</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0149</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>2.8043</v>
+        <v>4.6965</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0434</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1044,16 +1044,16 @@
         <v>0.3386</v>
       </c>
       <c r="F20" t="n">
-        <v>0.263</v>
+        <v>0.4086</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0128</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>72225.84420000001</v>
+        <v>154244.6426</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0386</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>